<commit_message>
Seguimos actualizando el examen
</commit_message>
<xml_diff>
--- a/11 Diseno Experimentos/Examen_2/data_papa.xlsx
+++ b/11 Diseno Experimentos/Examen_2/data_papa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\La Fuente Estadistic\Desktop\INLASER-LA FUENTE\General_Analytics\Maestria_UNSAAC\11 Diseno Experimentos\Examen_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE26C94E-DF3B-4EF0-9C50-D4C3E4E7650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C824F52-0CBE-4FA4-B4AB-BAFBC0C78ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E208DDC-3167-435F-8071-011810AD5BED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>formula</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>rendimiento</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>arcilloso</t>
+  </si>
+  <si>
+    <t>arenoso</t>
+  </si>
+  <si>
+    <t>franco arenoso</t>
   </si>
 </sst>
 </file>
@@ -397,10 +418,13 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -414,132 +438,132 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
       <c r="C4">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
       <c r="C5">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
       <c r="C6">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
+      <c r="A10" t="s">
         <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
       </c>
       <c r="C10">
         <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
       <c r="C11">
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
       </c>
       <c r="C12">
         <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
       <c r="C13">
         <v>190</v>

</xml_diff>